<commit_message>
minor tweaks to UI
</commit_message>
<xml_diff>
--- a/MIT_SpecificationInterface.xlsx
+++ b/MIT_SpecificationInterface.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltynes/repos/ESCALATE_Capture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D5169-20A2-B143-B862-654601767AB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="4" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="wellcount" localSheetId="0">'User Interface'!$E$6</definedName>
     <definedName name="wellcount">'WF1'!$D$7</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -145,6 +146,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Materials (</t>
     </r>
@@ -154,6 +156,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Chemicals</t>
     </r>
@@ -162,7 +165,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -178,6 +181,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chem</t>
     </r>
@@ -186,7 +190,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmin</t>
     </r>
@@ -199,6 +203,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chem</t>
     </r>
@@ -207,7 +212,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmax</t>
     </r>
@@ -227,7 +232,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent1_</t>
     </r>
@@ -238,6 +243,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -246,7 +252,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -263,7 +269,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -274,6 +280,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -287,7 +294,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent2_</t>
     </r>
@@ -298,6 +305,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -306,7 +314,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -353,7 +361,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent3_</t>
     </r>
@@ -364,6 +372,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -372,7 +381,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -389,7 +398,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Formula concentration of the 1st item in reagent3_chemical_list (</t>
     </r>
@@ -399,6 +408,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>mol / L of solvent</t>
     </r>
@@ -407,7 +417,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -427,7 +437,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent4_</t>
     </r>
@@ -438,6 +448,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -446,7 +457,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -463,7 +474,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Formula concentration of the 1st item in reagent4_chemical_list (</t>
     </r>
@@ -473,6 +484,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>mol / L of solvent</t>
     </r>
@@ -481,7 +493,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -495,7 +507,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Formula concentration of the 2nd item in reagent4_chemical_list (</t>
     </r>
@@ -505,6 +517,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>mol / L of solvent</t>
     </r>
@@ -513,7 +526,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -533,7 +546,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent5_</t>
     </r>
@@ -544,6 +557,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -552,7 +566,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -572,7 +586,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Formula concentration of the 1st item in reagent5_chemical_list (</t>
     </r>
@@ -582,6 +596,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>mol / L of solvent</t>
     </r>
@@ -590,7 +605,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -1119,6 +1134,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1127,7 +1143,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1209,6 +1225,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1217,7 +1234,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1251,6 +1268,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1259,7 +1277,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1325,6 +1343,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>mol / L of solvent</t>
     </r>
@@ -1333,7 +1352,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -1348,6 +1367,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>mol / L of solvent</t>
     </r>
@@ -1356,7 +1376,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -1365,7 +1385,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1379,12 +1399,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1392,35 +1414,41 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1441,6 +1469,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2490,11 +2519,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -3602,7 +3631,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="137">
-        <v>7.63</v>
+        <v>1.2</v>
       </c>
       <c r="F32" s="39">
         <v>5.6779999999999999</v>
@@ -3976,7 +4005,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="134">
-        <v>7</v>
+        <v>1.2</v>
       </c>
       <c r="F42" s="117">
         <v>9.0120000000000005</v>
@@ -15546,16 +15575,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" sqref="E6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
+    <dataValidation allowBlank="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" sqref="E6" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"MIT_PVLab, HC, LBL, dev"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please Check" prompt="Ensure that `ID` AND specify `Chemical list` for the same precursor, reagent, or dopant." sqref="A22"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activated vs Deactivated" prompt="Rows WITH `#` are &quot;deactivated&quot; and won't be read.  All other rows will be read by ESCALATE." sqref="A20"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please Check" prompt="Ensure that `ID` AND specify `Chemical list` for the same precursor, reagent, or dopant." sqref="A22" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activated vs Deactivated" prompt="Rows WITH `#` are &quot;deactivated&quot; and won't be read.  All other rows will be read by ESCALATE." sqref="A20" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H30" r:id="rId1"/>
-    <hyperlink ref="C18" location="'Manual Experiment Interface'!B2" display="Manual Experiments"/>
+    <hyperlink ref="H30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C18" location="'Manual Experiment Interface'!B2" display="Manual Experiments" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -15563,7 +15592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18041,7 +18070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -22556,7 +22585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W1030"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -23784,7 +23813,7 @@
       </c>
       <c r="D38" s="46">
         <f>'User Interface'!E32</f>
-        <v>7.63</v>
+        <v>1.2</v>
       </c>
       <c r="E38" s="39" t="s">
         <v>9</v>
@@ -24142,7 +24171,7 @@
       </c>
       <c r="D48" s="39">
         <f>'User Interface'!E42</f>
-        <v>7</v>
+        <v>1.2</v>
       </c>
       <c r="E48" s="39" t="s">
         <v>9</v>
@@ -32804,7 +32833,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="wellcount" prompt="MUST be sum of random_wellcount and fixed_wells" sqref="D7">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="wellcount" prompt="MUST be sum of random_wellcount and fixed_wells" sqref="D7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>SUM(#REF!,D18)</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
concentration v1 used for MIT, fixed devconfig
</commit_message>
<xml_diff>
--- a/MIT_SpecificationInterface.xlsx
+++ b/MIT_SpecificationInterface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE31C840-B56C-2F45-8057-E2F7A0A3A096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F32817-DF0F-624F-9EC9-B45B41A82DB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="51200" windowHeight="27540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="308">
   <si>
     <t>Comment</t>
   </si>
@@ -1444,6 +1444,9 @@
       <t>[M]</t>
     </r>
   </si>
+  <si>
+    <t>['MeNH3I','PbI2','1DMSO9DMF']</t>
+  </si>
 </sst>
 </file>
 
@@ -2621,7 +2624,7 @@
   <dimension ref="A1:AMK1024"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H42" sqref="H41:H42"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2634,8 +2637,8 @@
     <col min="6" max="6" width="44.6640625" customWidth="1"/>
     <col min="7" max="7" width="91.5" customWidth="1"/>
     <col min="8" max="8" width="92.1640625" customWidth="1"/>
-    <col min="9" max="26" width="8.83203125" hidden="1"/>
-    <col min="27" max="1025" width="14.5" hidden="1"/>
+    <col min="9" max="26" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="27" max="1025" width="14.5" hidden="1" customWidth="1"/>
     <col min="1026" max="16384" width="8.83203125" hidden="1"/>
   </cols>
   <sheetData>
@@ -3982,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="128" t="s">
-        <v>108</v>
+        <v>307</v>
       </c>
       <c r="F39" s="107" t="s">
         <v>208</v>
@@ -4087,7 +4090,9 @@
       <c r="Z41" s="6"/>
     </row>
     <row r="42" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="116"/>
+      <c r="A42" s="116" t="s">
+        <v>29</v>
+      </c>
       <c r="B42" s="70"/>
       <c r="C42" s="34" t="s">
         <v>126</v>
@@ -15704,7 +15709,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:XFD500"/>
+  <dimension ref="A1:XFC500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
@@ -28815,7 +28820,7 @@
       </c>
       <c r="D44" s="34" t="str">
         <f>'User Interface'!E39</f>
-        <v>['MeNH3I','PbI2','DMSO', 'DMF']</v>
+        <v>['MeNH3I','PbI2','1DMSO9DMF']</v>
       </c>
       <c r="E44" s="34" t="s">
         <v>18</v>
@@ -28951,9 +28956,9 @@
       <c r="W47" s="88"/>
     </row>
     <row r="48" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37">
+      <c r="A48" s="37" t="str">
         <f>'User Interface'!A42</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B48" s="75" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
MIT specification interface hotfixes, now includes additional actions and general language
</commit_message>
<xml_diff>
--- a/MIT_SpecificationInterface.xlsx
+++ b/MIT_SpecificationInterface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60458FF3-09A0-2940-83D7-CB7700198B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0799A0DC-8E03-B04B-85BE-2228E993AEA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="317">
   <si>
     <t>Comment</t>
   </si>
@@ -941,12 +941,6 @@
     <t>Dopant 1 Chemical List</t>
   </si>
   <si>
-    <t>Dopant 2 Chemical List</t>
-  </si>
-  <si>
-    <t>Capping Layer Chemical List</t>
-  </si>
-  <si>
     <t>['Chemical 1']</t>
   </si>
   <si>
@@ -1447,6 +1441,39 @@
   <si>
     <t>['MeNH3I','PbI2','1DMSO9DMF']</t>
   </si>
+  <si>
+    <t>Additional Solution (1) Chemical List</t>
+  </si>
+  <si>
+    <t>The specific names used in the templates designed by the lab can be changed without effecting code</t>
+  </si>
+  <si>
+    <t>Additional Solution (2) Chemical List</t>
+  </si>
+  <si>
+    <t>Additional_action_1_value</t>
+  </si>
+  <si>
+    <t>Additional_action_1_description</t>
+  </si>
+  <si>
+    <t>Additional_action_2_value</t>
+  </si>
+  <si>
+    <t>User defined additional action.  This column contains a numerical value (ex. 1000)</t>
+  </si>
+  <si>
+    <t>Description of the first additional action provided as a string with unit reference ex. vortex rate of sample (rpm)</t>
+  </si>
+  <si>
+    <t>Description of the additional action provided as a string with unit reference ex. vortex rate of sample (rpm)</t>
+  </si>
+  <si>
+    <t>stir rate (rpm)</t>
+  </si>
+  <si>
+    <t>stir rate duration (s)</t>
+  </si>
 </sst>
 </file>
 
@@ -1538,7 +1565,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1611,8 +1638,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEAF6"/>
+        <bgColor rgb="FFDEEAF6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1726,12 +1759,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2238,6 +2304,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2621,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK1024"/>
+  <dimension ref="A1:AMK1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2648,14 +2753,14 @@
       </c>
       <c r="B1" s="153"/>
       <c r="C1" s="154" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D1" s="155"/>
       <c r="E1" s="154" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F1" s="156" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G1" s="157" t="s">
         <v>5</v>
@@ -2764,10 +2869,10 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="148" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H4" s="162" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2832,7 +2937,7 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="149" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="6"/>
@@ -2902,7 +3007,7 @@
         <v>118</v>
       </c>
       <c r="G8" s="150" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="25"/>
@@ -2940,7 +3045,7 @@
         <v>117</v>
       </c>
       <c r="G9" s="150" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H9" s="24"/>
       <c r="I9" s="25"/>
@@ -3078,7 +3183,7 @@
         <v>118</v>
       </c>
       <c r="G13" s="138" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="6"/>
@@ -3116,7 +3221,7 @@
         <v>117</v>
       </c>
       <c r="G14" s="150" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="6"/>
@@ -3212,7 +3317,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="81" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="29"/>
@@ -3244,7 +3349,7 @@
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34"/>
@@ -3284,10 +3389,10 @@
       <c r="E20" s="125"/>
       <c r="F20" s="34"/>
       <c r="G20" s="143" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H20" s="151" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -3323,13 +3428,13 @@
         <v>166</v>
       </c>
       <c r="F21" s="78" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G21" s="143" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H21" s="152" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -3390,7 +3495,7 @@
       </c>
       <c r="B23" s="70"/>
       <c r="C23" s="107" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D23" s="35" t="s">
         <v>2</v>
@@ -3428,7 +3533,7 @@
       </c>
       <c r="B24" s="70"/>
       <c r="C24" s="107" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D24" s="35" t="s">
         <v>2</v>
@@ -3466,7 +3571,7 @@
       </c>
       <c r="B25" s="70"/>
       <c r="C25" s="107" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D25" s="108" t="s">
         <v>2</v>
@@ -3502,7 +3607,7 @@
       </c>
       <c r="B26" s="70"/>
       <c r="C26" s="75" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D26" s="35" t="s">
         <v>2</v>
@@ -3538,7 +3643,7 @@
       </c>
       <c r="B27" s="70"/>
       <c r="C27" s="75" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D27" s="35" t="s">
         <v>2</v>
@@ -3574,7 +3679,7 @@
       </c>
       <c r="B28" s="70"/>
       <c r="C28" s="75" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>2</v>
@@ -3647,13 +3752,13 @@
         <v>121</v>
       </c>
       <c r="F30" s="107" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G30" s="143" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H30" s="113" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -3690,7 +3795,7 @@
         <v>1.234</v>
       </c>
       <c r="G31" s="143" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H31" s="36"/>
       <c r="I31" s="6"/>
@@ -3728,7 +3833,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G32" s="143" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H32" s="36"/>
       <c r="I32" s="6"/>
@@ -3984,13 +4089,13 @@
         <v>2</v>
       </c>
       <c r="E39" s="128" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F39" s="107" t="s">
         <v>208</v>
       </c>
       <c r="G39" s="143" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H39" s="36"/>
       <c r="I39" s="6"/>
@@ -4028,7 +4133,7 @@
         <v>1.234</v>
       </c>
       <c r="G40" s="143" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="6"/>
@@ -4066,7 +4171,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G41" s="143" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H41" s="36"/>
       <c r="I41" s="6"/>
@@ -4106,7 +4211,7 @@
         <v>9.0120000000000005</v>
       </c>
       <c r="G42" s="143" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="6"/>
@@ -4331,10 +4436,10 @@
         <v>121</v>
       </c>
       <c r="F48" s="107" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G48" s="143" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H48" s="39"/>
       <c r="I48" s="6"/>
@@ -4374,7 +4479,7 @@
         <v>1.234</v>
       </c>
       <c r="G49" s="143" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H49" s="36"/>
       <c r="I49" s="6"/>
@@ -4414,7 +4519,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G50" s="143" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H50" s="36"/>
       <c r="I50" s="6"/>
@@ -4678,7 +4783,7 @@
         <v>208</v>
       </c>
       <c r="G57" s="143" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H57" s="113" t="s">
         <v>149</v>
@@ -4720,7 +4825,7 @@
         <v>1.234</v>
       </c>
       <c r="G58" s="143" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H58" s="44"/>
       <c r="I58" s="6"/>
@@ -4760,7 +4865,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G59" s="143" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H59" s="44"/>
       <c r="I59" s="6"/>
@@ -4800,7 +4905,7 @@
         <v>9.0120000000000005</v>
       </c>
       <c r="G60" s="143" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H60" s="39"/>
       <c r="I60" s="6"/>
@@ -5025,10 +5130,10 @@
         <v>121</v>
       </c>
       <c r="F66" s="107" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G66" s="143" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H66" s="36"/>
       <c r="I66" s="6"/>
@@ -5068,7 +5173,7 @@
         <v>1.234</v>
       </c>
       <c r="G67" s="143" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H67" s="36"/>
       <c r="I67" s="6"/>
@@ -5108,7 +5213,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G68" s="143" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="6"/>
@@ -5344,7 +5449,7 @@
         <v>7</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>225</v>
+        <v>306</v>
       </c>
       <c r="D75" s="67" t="s">
         <v>2</v>
@@ -5353,12 +5458,14 @@
         <v>121</v>
       </c>
       <c r="F75" s="107" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G75" s="143" t="s">
-        <v>301</v>
-      </c>
-      <c r="H75" s="36"/>
+        <v>299</v>
+      </c>
+      <c r="H75" s="113" t="s">
+        <v>307</v>
+      </c>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
@@ -5396,7 +5503,7 @@
         <v>1.234</v>
       </c>
       <c r="G76" s="143" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H76" s="36"/>
       <c r="I76" s="6"/>
@@ -5436,7 +5543,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G77" s="143" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H77" s="36"/>
       <c r="I77" s="6"/>
@@ -5673,7 +5780,7 @@
         <v>8</v>
       </c>
       <c r="C84" s="75" t="s">
-        <v>226</v>
+        <v>308</v>
       </c>
       <c r="D84" s="67" t="s">
         <v>2</v>
@@ -5682,12 +5789,14 @@
         <v>121</v>
       </c>
       <c r="F84" s="107" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G84" s="143" t="s">
-        <v>302</v>
-      </c>
-      <c r="H84" s="36"/>
+        <v>300</v>
+      </c>
+      <c r="H84" s="113" t="s">
+        <v>307</v>
+      </c>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
@@ -5725,7 +5834,7 @@
         <v>1.234</v>
       </c>
       <c r="G85" s="143" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H85" s="36"/>
       <c r="I85" s="6"/>
@@ -5765,7 +5874,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G86" s="143" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H86" s="36"/>
       <c r="I86" s="6"/>
@@ -6267,277 +6376,389 @@
       <c r="Y99" s="6"/>
       <c r="Z99" s="6"/>
     </row>
-    <row r="100" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="52" t="s">
+    <row r="100" spans="1:26" s="89" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="B100" s="52"/>
-      <c r="C100" s="53" t="s">
+      <c r="B100" s="51"/>
+      <c r="C100" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="D100" s="54" t="s">
+      <c r="D100" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="131" t="s">
+      <c r="E100" s="169" t="s">
         <v>163</v>
       </c>
-      <c r="F100" s="53"/>
-      <c r="G100" s="146" t="s">
+      <c r="F100" s="102"/>
+      <c r="G100" s="170" t="s">
         <v>88</v>
       </c>
-      <c r="H100" s="55" t="s">
+      <c r="H100" s="171" t="s">
         <v>89</v>
       </c>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-      <c r="S100" s="1"/>
-      <c r="T100" s="1"/>
-      <c r="U100" s="1"/>
-      <c r="V100" s="1"/>
-      <c r="W100" s="1"/>
-      <c r="X100" s="1"/>
-      <c r="Y100" s="1"/>
-      <c r="Z100" s="1"/>
-    </row>
-    <row r="101" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="69" t="s">
-        <v>154</v>
-      </c>
-      <c r="B101" s="69"/>
-      <c r="C101" s="48"/>
-      <c r="D101" s="49"/>
-      <c r="E101" s="130"/>
-      <c r="F101" s="48"/>
-      <c r="G101" s="145"/>
-      <c r="H101" s="50"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="6"/>
-      <c r="K101" s="6"/>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6"/>
-      <c r="N101" s="6"/>
-      <c r="O101" s="6"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="6"/>
-      <c r="S101" s="6"/>
-      <c r="T101" s="6"/>
-      <c r="U101" s="6"/>
-      <c r="V101" s="6"/>
-      <c r="W101" s="6"/>
-      <c r="X101" s="6"/>
-      <c r="Y101" s="6"/>
-      <c r="Z101" s="6"/>
+      <c r="I100" s="88"/>
+      <c r="J100" s="88"/>
+      <c r="K100" s="88"/>
+      <c r="L100" s="88"/>
+      <c r="M100" s="88"/>
+      <c r="N100" s="88"/>
+      <c r="O100" s="88"/>
+      <c r="P100" s="88"/>
+      <c r="Q100" s="88"/>
+      <c r="R100" s="88"/>
+      <c r="S100" s="88"/>
+      <c r="T100" s="88"/>
+      <c r="U100" s="88"/>
+      <c r="V100" s="88"/>
+      <c r="W100" s="88"/>
+      <c r="X100" s="88"/>
+      <c r="Y100" s="88"/>
+      <c r="Z100" s="88"/>
+    </row>
+    <row r="101" spans="1:26" s="89" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="51"/>
+      <c r="B101" s="51"/>
+      <c r="C101" s="176" t="s">
+        <v>309</v>
+      </c>
+      <c r="D101" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="E101" s="173">
+        <v>0</v>
+      </c>
+      <c r="F101" s="173">
+        <v>100</v>
+      </c>
+      <c r="G101" s="179" t="s">
+        <v>312</v>
+      </c>
+      <c r="H101" s="177"/>
+      <c r="I101" s="88"/>
+      <c r="J101" s="88"/>
+      <c r="K101" s="88"/>
+      <c r="L101" s="88"/>
+      <c r="M101" s="88"/>
+      <c r="N101" s="88"/>
+      <c r="O101" s="88"/>
+      <c r="P101" s="88"/>
+      <c r="Q101" s="88"/>
+      <c r="R101" s="88"/>
+      <c r="S101" s="88"/>
+      <c r="T101" s="88"/>
+      <c r="U101" s="88"/>
+      <c r="V101" s="88"/>
+      <c r="W101" s="88"/>
+      <c r="X101" s="88"/>
+      <c r="Y101" s="88"/>
+      <c r="Z101" s="88"/>
     </row>
     <row r="102" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="51"/>
       <c r="B102" s="51"/>
-      <c r="C102" s="77" t="s">
-        <v>164</v>
-      </c>
-      <c r="D102" s="49" t="s">
+      <c r="C102" s="176" t="s">
+        <v>310</v>
+      </c>
+      <c r="D102" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="E102" s="130">
-        <v>45</v>
-      </c>
-      <c r="F102" s="48">
-        <v>45</v>
-      </c>
-      <c r="G102" s="147" t="s">
-        <v>165</v>
-      </c>
-      <c r="H102" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="6"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
-      <c r="N102" s="6"/>
-      <c r="O102" s="6"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="6"/>
-      <c r="S102" s="6"/>
-      <c r="T102" s="6"/>
-      <c r="U102" s="6"/>
-      <c r="V102" s="6"/>
-      <c r="W102" s="6"/>
-      <c r="X102" s="6"/>
-      <c r="Y102" s="6"/>
-      <c r="Z102" s="6"/>
+      <c r="E102" s="173">
+        <v>0</v>
+      </c>
+      <c r="F102" s="176" t="s">
+        <v>315</v>
+      </c>
+      <c r="G102" s="180" t="s">
+        <v>314</v>
+      </c>
+      <c r="H102" s="175"/>
+      <c r="I102" s="88"/>
+      <c r="J102" s="88"/>
+      <c r="K102" s="88"/>
+      <c r="L102" s="88"/>
+      <c r="M102" s="88"/>
+      <c r="N102" s="88"/>
+      <c r="O102" s="88"/>
+      <c r="P102" s="88"/>
+      <c r="Q102" s="88"/>
+      <c r="R102" s="88"/>
+      <c r="S102" s="88"/>
+      <c r="T102" s="88"/>
+      <c r="U102" s="88"/>
+      <c r="V102" s="88"/>
+      <c r="W102" s="88"/>
+      <c r="X102" s="88"/>
+      <c r="Y102" s="88"/>
+      <c r="Z102" s="88"/>
     </row>
     <row r="103" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="51"/>
       <c r="B103" s="51"/>
-      <c r="C103" s="48" t="s">
+      <c r="C103" s="176" t="s">
+        <v>311</v>
+      </c>
+      <c r="D103" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="E103" s="173">
+        <v>0</v>
+      </c>
+      <c r="F103" s="173">
+        <v>1200</v>
+      </c>
+      <c r="G103" s="179" t="s">
+        <v>312</v>
+      </c>
+      <c r="H103" s="175"/>
+      <c r="I103" s="88"/>
+      <c r="J103" s="88"/>
+      <c r="K103" s="88"/>
+      <c r="L103" s="88"/>
+      <c r="M103" s="88"/>
+      <c r="N103" s="88"/>
+      <c r="O103" s="88"/>
+      <c r="P103" s="88"/>
+      <c r="Q103" s="88"/>
+      <c r="R103" s="88"/>
+      <c r="S103" s="88"/>
+      <c r="T103" s="88"/>
+      <c r="U103" s="88"/>
+      <c r="V103" s="88"/>
+      <c r="W103" s="88"/>
+      <c r="X103" s="88"/>
+      <c r="Y103" s="88"/>
+      <c r="Z103" s="88"/>
+    </row>
+    <row r="104" spans="1:26" s="172" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="52"/>
+      <c r="B104" s="52"/>
+      <c r="C104" s="178" t="s">
+        <v>310</v>
+      </c>
+      <c r="D104" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="131">
+        <v>0</v>
+      </c>
+      <c r="F104" s="178" t="s">
+        <v>316</v>
+      </c>
+      <c r="G104" s="181" t="s">
+        <v>313</v>
+      </c>
+      <c r="H104" s="55"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+      <c r="Y104" s="1"/>
+      <c r="Z104" s="1"/>
+    </row>
+    <row r="105" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="69" t="s">
+        <v>154</v>
+      </c>
+      <c r="B105" s="69"/>
+      <c r="C105" s="48"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="130"/>
+      <c r="F105" s="48"/>
+      <c r="G105" s="145"/>
+      <c r="H105" s="50"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="6"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="6"/>
+      <c r="S105" s="6"/>
+      <c r="T105" s="6"/>
+      <c r="U105" s="6"/>
+      <c r="V105" s="6"/>
+      <c r="W105" s="6"/>
+      <c r="X105" s="6"/>
+      <c r="Y105" s="6"/>
+      <c r="Z105" s="6"/>
+    </row>
+    <row r="106" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="51"/>
+      <c r="B106" s="51"/>
+      <c r="C106" s="77" t="s">
+        <v>164</v>
+      </c>
+      <c r="D106" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E106" s="130">
+        <v>45</v>
+      </c>
+      <c r="F106" s="48">
+        <v>45</v>
+      </c>
+      <c r="G106" s="147" t="s">
+        <v>165</v>
+      </c>
+      <c r="H106" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
+      <c r="P106" s="6"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="6"/>
+      <c r="S106" s="6"/>
+      <c r="T106" s="6"/>
+      <c r="U106" s="6"/>
+      <c r="V106" s="6"/>
+      <c r="W106" s="6"/>
+      <c r="X106" s="6"/>
+      <c r="Y106" s="6"/>
+      <c r="Z106" s="6"/>
+    </row>
+    <row r="107" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="51"/>
+      <c r="B107" s="51"/>
+      <c r="C107" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="D103" s="49" t="s">
+      <c r="D107" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E103" s="130">
+      <c r="E107" s="130">
         <v>25</v>
       </c>
-      <c r="F103" s="48">
+      <c r="F107" s="48">
         <v>75</v>
       </c>
-      <c r="G103" s="145" t="s">
+      <c r="G107" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="H103" s="50" t="s">
+      <c r="H107" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="I103" s="6"/>
-      <c r="J103" s="6"/>
-      <c r="K103" s="6"/>
-      <c r="L103" s="6"/>
-      <c r="M103" s="6"/>
-      <c r="N103" s="6"/>
-      <c r="O103" s="6"/>
-      <c r="P103" s="6"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="6"/>
-      <c r="S103" s="6"/>
-      <c r="T103" s="6"/>
-      <c r="U103" s="6"/>
-      <c r="V103" s="6"/>
-      <c r="W103" s="6"/>
-      <c r="X103" s="6"/>
-      <c r="Y103" s="6"/>
-      <c r="Z103" s="6"/>
-    </row>
-    <row r="104" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="51"/>
-      <c r="B104" s="51"/>
-      <c r="C104" s="48" t="s">
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
+      <c r="O107" s="6"/>
+      <c r="P107" s="6"/>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="6"/>
+      <c r="S107" s="6"/>
+      <c r="T107" s="6"/>
+      <c r="U107" s="6"/>
+      <c r="V107" s="6"/>
+      <c r="W107" s="6"/>
+      <c r="X107" s="6"/>
+      <c r="Y107" s="6"/>
+      <c r="Z107" s="6"/>
+    </row>
+    <row r="108" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="51"/>
+      <c r="B108" s="51"/>
+      <c r="C108" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="D104" s="49" t="s">
+      <c r="D108" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E104" s="130">
+      <c r="E108" s="130">
         <v>450</v>
       </c>
-      <c r="F104" s="48">
+      <c r="F108" s="48">
         <v>450</v>
       </c>
-      <c r="G104" s="145" t="s">
+      <c r="G108" s="145" t="s">
         <v>96</v>
       </c>
-      <c r="H104" s="50" t="s">
+      <c r="H108" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="I104" s="6"/>
-      <c r="J104" s="6"/>
-      <c r="K104" s="6"/>
-      <c r="L104" s="6"/>
-      <c r="M104" s="6"/>
-      <c r="N104" s="6"/>
-      <c r="O104" s="6"/>
-      <c r="P104" s="6"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="6"/>
-      <c r="S104" s="6"/>
-      <c r="T104" s="6"/>
-      <c r="U104" s="6"/>
-      <c r="V104" s="6"/>
-      <c r="W104" s="6"/>
-      <c r="X104" s="6"/>
-      <c r="Y104" s="6"/>
-      <c r="Z104" s="6"/>
-    </row>
-    <row r="105" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="52"/>
-      <c r="B105" s="52"/>
-      <c r="C105" s="53" t="s">
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
+      <c r="P108" s="6"/>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="6"/>
+      <c r="S108" s="6"/>
+      <c r="T108" s="6"/>
+      <c r="U108" s="6"/>
+      <c r="V108" s="6"/>
+      <c r="W108" s="6"/>
+      <c r="X108" s="6"/>
+      <c r="Y108" s="6"/>
+      <c r="Z108" s="6"/>
+    </row>
+    <row r="109" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="52"/>
+      <c r="B109" s="52"/>
+      <c r="C109" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="D105" s="54" t="s">
+      <c r="D109" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="132">
+      <c r="E109" s="132">
         <v>3600</v>
       </c>
-      <c r="F105" s="53">
+      <c r="F109" s="53">
         <v>3600</v>
       </c>
-      <c r="G105" s="146" t="s">
+      <c r="G109" s="146" t="s">
         <v>98</v>
       </c>
-      <c r="H105" s="55" t="s">
+      <c r="H109" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
-      <c r="N105" s="1"/>
-      <c r="O105" s="1"/>
-      <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
-      <c r="S105" s="1"/>
-      <c r="T105" s="1"/>
-      <c r="U105" s="1"/>
-      <c r="V105" s="1"/>
-      <c r="W105" s="1"/>
-      <c r="X105" s="1"/>
-      <c r="Y105" s="1"/>
-      <c r="Z105" s="1"/>
-    </row>
-    <row r="106" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="56"/>
-      <c r="B106" s="56"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="58"/>
-      <c r="E106" s="57"/>
-      <c r="F106" s="57"/>
-      <c r="G106" s="59"/>
-      <c r="H106" s="60"/>
-    </row>
-    <row r="107" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="56"/>
-      <c r="B107" s="56"/>
-      <c r="C107" s="57"/>
-      <c r="D107" s="58"/>
-      <c r="E107" s="57"/>
-      <c r="F107" s="57"/>
-      <c r="G107" s="59"/>
-      <c r="H107" s="60"/>
-    </row>
-    <row r="108" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="56"/>
-      <c r="B108" s="56"/>
-      <c r="C108" s="57"/>
-      <c r="D108" s="58"/>
-      <c r="E108" s="57"/>
-      <c r="F108" s="57"/>
-      <c r="G108" s="59"/>
-      <c r="H108" s="60"/>
-    </row>
-    <row r="109" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="56"/>
-      <c r="B109" s="56"/>
-      <c r="C109" s="57"/>
-      <c r="D109" s="58"/>
-      <c r="E109" s="57"/>
-      <c r="F109" s="57"/>
-      <c r="G109" s="59"/>
-      <c r="H109" s="60"/>
-    </row>
-    <row r="110" spans="1:26" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+      <c r="S109" s="1"/>
+      <c r="T109" s="1"/>
+      <c r="U109" s="1"/>
+      <c r="V109" s="1"/>
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
+      <c r="Y109" s="1"/>
+      <c r="Z109" s="1"/>
+    </row>
+    <row r="110" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="56"/>
       <c r="B110" s="56"/>
       <c r="C110" s="57"/>
@@ -15686,6 +15907,46 @@
       <c r="F1024" s="57"/>
       <c r="G1024" s="59"/>
       <c r="H1024" s="60"/>
+    </row>
+    <row r="1025" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1025" s="56"/>
+      <c r="B1025" s="56"/>
+      <c r="C1025" s="57"/>
+      <c r="D1025" s="58"/>
+      <c r="E1025" s="57"/>
+      <c r="F1025" s="57"/>
+      <c r="G1025" s="59"/>
+      <c r="H1025" s="60"/>
+    </row>
+    <row r="1026" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1026" s="56"/>
+      <c r="B1026" s="56"/>
+      <c r="C1026" s="57"/>
+      <c r="D1026" s="58"/>
+      <c r="E1026" s="57"/>
+      <c r="F1026" s="57"/>
+      <c r="G1026" s="59"/>
+      <c r="H1026" s="60"/>
+    </row>
+    <row r="1027" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1027" s="56"/>
+      <c r="B1027" s="56"/>
+      <c r="C1027" s="57"/>
+      <c r="D1027" s="58"/>
+      <c r="E1027" s="57"/>
+      <c r="F1027" s="57"/>
+      <c r="G1027" s="59"/>
+      <c r="H1027" s="60"/>
+    </row>
+    <row r="1028" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1028" s="56"/>
+      <c r="B1028" s="56"/>
+      <c r="C1028" s="57"/>
+      <c r="D1028" s="58"/>
+      <c r="E1028" s="57"/>
+      <c r="F1028" s="57"/>
+      <c r="G1028" s="59"/>
+      <c r="H1028" s="60"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -15841,7 +16102,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="166" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C4" s="164">
         <v>150</v>
@@ -27521,10 +27782,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:W1030"/>
+  <dimension ref="A1:W1034"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28383,7 +28644,7 @@
         <v>#</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C28" s="35" t="s">
         <v>2</v>
@@ -28420,7 +28681,7 @@
         <v>#</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C29" s="35" t="s">
         <v>2</v>
@@ -28457,7 +28718,7 @@
         <v>#</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C30" s="35" t="s">
         <v>2</v>
@@ -28494,7 +28755,7 @@
         <v>#</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C31" s="35" t="s">
         <v>2</v>
@@ -28531,7 +28792,7 @@
         <v>#</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C32" s="35" t="s">
         <v>2</v>
@@ -28568,7 +28829,7 @@
         <v>#</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>2</v>
@@ -28778,7 +29039,7 @@
         <v>#</v>
       </c>
       <c r="B39" s="75" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C39" s="35" t="s">
         <v>2</v>
@@ -29420,7 +29681,7 @@
         <v>#</v>
       </c>
       <c r="B57" s="75" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C57" s="35" t="s">
         <v>2</v>
@@ -29704,7 +29965,7 @@
         <v>#</v>
       </c>
       <c r="B65" s="112" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C65" s="35" t="s">
         <v>2</v>
@@ -29741,7 +30002,7 @@
         <v>#</v>
       </c>
       <c r="B66" s="75" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C66" s="35" t="s">
         <v>2</v>
@@ -29914,7 +30175,7 @@
         <v>#</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C71" s="35" t="s">
         <v>2</v>
@@ -29988,7 +30249,7 @@
         <v>#</v>
       </c>
       <c r="B73" s="112" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C73" s="35" t="s">
         <v>2</v>
@@ -30025,7 +30286,7 @@
         <v>#</v>
       </c>
       <c r="B74" s="112" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C74" s="35" t="s">
         <v>2</v>
@@ -30062,7 +30323,7 @@
         <v>#</v>
       </c>
       <c r="B75" s="75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C75" s="35" t="s">
         <v>2</v>
@@ -30099,7 +30360,7 @@
         <v>#</v>
       </c>
       <c r="B76" s="75" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C76" s="35" t="s">
         <v>2</v>
@@ -30136,7 +30397,7 @@
         <v>#</v>
       </c>
       <c r="B77" s="75" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C77" s="35" t="s">
         <v>2</v>
@@ -30173,7 +30434,7 @@
         <v>#</v>
       </c>
       <c r="B78" s="75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C78" s="35" t="s">
         <v>2</v>
@@ -30235,7 +30496,7 @@
         <v>#</v>
       </c>
       <c r="B80" s="75" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C80" s="35" t="s">
         <v>2</v>
@@ -30309,7 +30570,7 @@
         <v>#</v>
       </c>
       <c r="B82" s="112" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C82" s="35" t="s">
         <v>2</v>
@@ -30346,7 +30607,7 @@
         <v>#</v>
       </c>
       <c r="B83" s="112" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C83" s="35" t="s">
         <v>2</v>
@@ -30383,7 +30644,7 @@
         <v>#</v>
       </c>
       <c r="B84" s="75" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C84" s="35" t="s">
         <v>2</v>
@@ -30420,7 +30681,7 @@
         <v>#</v>
       </c>
       <c r="B85" s="75" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C85" s="35" t="s">
         <v>2</v>
@@ -30457,7 +30718,7 @@
         <v>#</v>
       </c>
       <c r="B86" s="75" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C86" s="35" t="s">
         <v>2</v>
@@ -30494,7 +30755,7 @@
         <v>#</v>
       </c>
       <c r="B87" s="75" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C87" s="35" t="s">
         <v>2</v>
@@ -30556,7 +30817,7 @@
         <v>#</v>
       </c>
       <c r="B89" s="75" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C89" s="35" t="s">
         <v>2</v>
@@ -30593,7 +30854,7 @@
         <v>#</v>
       </c>
       <c r="B90" s="78" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C90" s="43" t="s">
         <v>2</v>
@@ -30630,7 +30891,7 @@
         <v>#</v>
       </c>
       <c r="B91" s="112" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C91" s="35" t="s">
         <v>2</v>
@@ -30667,7 +30928,7 @@
         <v>#</v>
       </c>
       <c r="B92" s="112" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C92" s="35" t="s">
         <v>2</v>
@@ -30704,7 +30965,7 @@
         <v>#</v>
       </c>
       <c r="B93" s="75" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C93" s="35" t="s">
         <v>2</v>
@@ -30741,7 +31002,7 @@
         <v>#</v>
       </c>
       <c r="B94" s="75" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C94" s="35" t="s">
         <v>2</v>
@@ -30778,7 +31039,7 @@
         <v>#</v>
       </c>
       <c r="B95" s="75" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C95" s="35" t="s">
         <v>2</v>
@@ -30815,7 +31076,7 @@
         <v>#</v>
       </c>
       <c r="B96" s="75" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C96" s="35" t="s">
         <v>2</v>
@@ -31171,13 +31432,20 @@
       <c r="W106" s="88"/>
     </row>
     <row r="107" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B107" s="48"/>
-      <c r="C107" s="49"/>
-      <c r="D107" s="48"/>
-      <c r="E107" s="48"/>
+      <c r="A107" s="51"/>
+      <c r="B107" s="176" t="s">
+        <v>309</v>
+      </c>
+      <c r="C107" s="174" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" s="173">
+        <f>'User Interface'!E101</f>
+        <v>0</v>
+      </c>
+      <c r="E107" s="77" t="s">
+        <v>11</v>
+      </c>
       <c r="F107" s="88"/>
       <c r="G107" s="88"/>
       <c r="H107" s="88"/>
@@ -31199,18 +31467,18 @@
     </row>
     <row r="108" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="51"/>
-      <c r="B108" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="C108" s="49" t="s">
+      <c r="B108" s="176" t="s">
+        <v>310</v>
+      </c>
+      <c r="C108" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="D108" s="48">
+      <c r="D108" s="173">
         <f>'User Interface'!E102</f>
-        <v>45</v>
-      </c>
-      <c r="E108" s="48" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E108" s="77" t="s">
+        <v>13</v>
       </c>
       <c r="F108" s="88"/>
       <c r="G108" s="88"/>
@@ -31233,17 +31501,17 @@
     </row>
     <row r="109" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="51"/>
-      <c r="B109" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C109" s="49" t="s">
+      <c r="B109" s="176" t="s">
+        <v>311</v>
+      </c>
+      <c r="C109" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="D109" s="48">
+      <c r="D109" s="173">
         <f>'User Interface'!E103</f>
-        <v>25</v>
-      </c>
-      <c r="E109" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="77" t="s">
         <v>11</v>
       </c>
       <c r="F109" s="88"/>
@@ -31267,18 +31535,18 @@
     </row>
     <row r="110" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="51"/>
-      <c r="B110" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="C110" s="49" t="s">
+      <c r="B110" s="77" t="s">
+        <v>310</v>
+      </c>
+      <c r="C110" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="D110" s="48">
+      <c r="D110" s="173">
         <f>'User Interface'!E104</f>
-        <v>450</v>
-      </c>
-      <c r="E110" s="48" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E110" s="77" t="s">
+        <v>13</v>
       </c>
       <c r="F110" s="88"/>
       <c r="G110" s="88"/>
@@ -31300,20 +31568,13 @@
       <c r="W110" s="88"/>
     </row>
     <row r="111" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="51"/>
-      <c r="B111" s="102" t="s">
-        <v>97</v>
-      </c>
-      <c r="C111" s="103" t="s">
-        <v>2</v>
-      </c>
-      <c r="D111" s="48">
-        <f>'User Interface'!E105</f>
-        <v>3600</v>
-      </c>
-      <c r="E111" s="102" t="s">
-        <v>11</v>
-      </c>
+      <c r="A111" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B111" s="48"/>
+      <c r="C111" s="49"/>
+      <c r="D111" s="48"/>
+      <c r="E111" s="48"/>
       <c r="F111" s="88"/>
       <c r="G111" s="88"/>
       <c r="H111" s="88"/>
@@ -31334,118 +31595,226 @@
       <c r="W111" s="88"/>
     </row>
     <row r="112" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="104"/>
-      <c r="B112" s="105"/>
-      <c r="C112" s="106"/>
-      <c r="D112" s="105"/>
-      <c r="E112" s="105"/>
-    </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="104"/>
-      <c r="B113" s="105"/>
-      <c r="C113" s="106"/>
-      <c r="D113" s="105"/>
-      <c r="E113" s="105"/>
-    </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="104"/>
-      <c r="B114" s="105"/>
-      <c r="C114" s="106"/>
-      <c r="D114" s="105"/>
-      <c r="E114" s="105"/>
-    </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="104"/>
-      <c r="B115" s="105"/>
-      <c r="C115" s="106"/>
-      <c r="D115" s="105"/>
-      <c r="E115" s="105"/>
-    </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="51"/>
+      <c r="B112" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C112" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" s="48">
+        <f>'User Interface'!E106</f>
+        <v>45</v>
+      </c>
+      <c r="E112" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" s="88"/>
+      <c r="G112" s="88"/>
+      <c r="H112" s="88"/>
+      <c r="I112" s="88"/>
+      <c r="J112" s="88"/>
+      <c r="K112" s="88"/>
+      <c r="L112" s="88"/>
+      <c r="M112" s="88"/>
+      <c r="N112" s="88"/>
+      <c r="O112" s="88"/>
+      <c r="P112" s="88"/>
+      <c r="Q112" s="88"/>
+      <c r="R112" s="88"/>
+      <c r="S112" s="88"/>
+      <c r="T112" s="88"/>
+      <c r="U112" s="88"/>
+      <c r="V112" s="88"/>
+      <c r="W112" s="88"/>
+    </row>
+    <row r="113" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="51"/>
+      <c r="B113" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C113" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" s="48">
+        <f>'User Interface'!E107</f>
+        <v>25</v>
+      </c>
+      <c r="E113" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" s="88"/>
+      <c r="G113" s="88"/>
+      <c r="H113" s="88"/>
+      <c r="I113" s="88"/>
+      <c r="J113" s="88"/>
+      <c r="K113" s="88"/>
+      <c r="L113" s="88"/>
+      <c r="M113" s="88"/>
+      <c r="N113" s="88"/>
+      <c r="O113" s="88"/>
+      <c r="P113" s="88"/>
+      <c r="Q113" s="88"/>
+      <c r="R113" s="88"/>
+      <c r="S113" s="88"/>
+      <c r="T113" s="88"/>
+      <c r="U113" s="88"/>
+      <c r="V113" s="88"/>
+      <c r="W113" s="88"/>
+    </row>
+    <row r="114" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="51"/>
+      <c r="B114" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C114" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" s="48">
+        <f>'User Interface'!E108</f>
+        <v>450</v>
+      </c>
+      <c r="E114" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="88"/>
+      <c r="G114" s="88"/>
+      <c r="H114" s="88"/>
+      <c r="I114" s="88"/>
+      <c r="J114" s="88"/>
+      <c r="K114" s="88"/>
+      <c r="L114" s="88"/>
+      <c r="M114" s="88"/>
+      <c r="N114" s="88"/>
+      <c r="O114" s="88"/>
+      <c r="P114" s="88"/>
+      <c r="Q114" s="88"/>
+      <c r="R114" s="88"/>
+      <c r="S114" s="88"/>
+      <c r="T114" s="88"/>
+      <c r="U114" s="88"/>
+      <c r="V114" s="88"/>
+      <c r="W114" s="88"/>
+    </row>
+    <row r="115" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="51"/>
+      <c r="B115" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="C115" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" s="48">
+        <f>'User Interface'!E109</f>
+        <v>3600</v>
+      </c>
+      <c r="E115" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="88"/>
+      <c r="G115" s="88"/>
+      <c r="H115" s="88"/>
+      <c r="I115" s="88"/>
+      <c r="J115" s="88"/>
+      <c r="K115" s="88"/>
+      <c r="L115" s="88"/>
+      <c r="M115" s="88"/>
+      <c r="N115" s="88"/>
+      <c r="O115" s="88"/>
+      <c r="P115" s="88"/>
+      <c r="Q115" s="88"/>
+      <c r="R115" s="88"/>
+      <c r="S115" s="88"/>
+      <c r="T115" s="88"/>
+      <c r="U115" s="88"/>
+      <c r="V115" s="88"/>
+      <c r="W115" s="88"/>
+    </row>
+    <row r="116" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="104"/>
       <c r="B116" s="105"/>
       <c r="C116" s="106"/>
       <c r="D116" s="105"/>
       <c r="E116" s="105"/>
     </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="104"/>
       <c r="B117" s="105"/>
       <c r="C117" s="106"/>
       <c r="D117" s="105"/>
       <c r="E117" s="105"/>
     </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="104"/>
       <c r="B118" s="105"/>
       <c r="C118" s="106"/>
       <c r="D118" s="105"/>
       <c r="E118" s="105"/>
     </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="104"/>
       <c r="B119" s="105"/>
       <c r="C119" s="106"/>
       <c r="D119" s="105"/>
       <c r="E119" s="105"/>
     </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="104"/>
       <c r="B120" s="105"/>
       <c r="C120" s="106"/>
       <c r="D120" s="105"/>
       <c r="E120" s="105"/>
     </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="104"/>
       <c r="B121" s="105"/>
       <c r="C121" s="106"/>
       <c r="D121" s="105"/>
       <c r="E121" s="105"/>
     </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="104"/>
       <c r="B122" s="105"/>
       <c r="C122" s="106"/>
       <c r="D122" s="105"/>
       <c r="E122" s="105"/>
     </row>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="104"/>
       <c r="B123" s="105"/>
       <c r="C123" s="106"/>
       <c r="D123" s="105"/>
       <c r="E123" s="105"/>
     </row>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="104"/>
       <c r="B124" s="105"/>
       <c r="C124" s="106"/>
       <c r="D124" s="105"/>
       <c r="E124" s="105"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="104"/>
       <c r="B125" s="105"/>
       <c r="C125" s="106"/>
       <c r="D125" s="105"/>
       <c r="E125" s="105"/>
     </row>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="104"/>
       <c r="B126" s="105"/>
       <c r="C126" s="106"/>
       <c r="D126" s="105"/>
       <c r="E126" s="105"/>
     </row>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="104"/>
       <c r="B127" s="105"/>
       <c r="C127" s="106"/>
       <c r="D127" s="105"/>
       <c r="E127" s="105"/>
     </row>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="104"/>
       <c r="B128" s="105"/>
       <c r="C128" s="106"/>
@@ -37765,6 +38134,34 @@
       <c r="C1030" s="106"/>
       <c r="D1030" s="105"/>
       <c r="E1030" s="105"/>
+    </row>
+    <row r="1031" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1031" s="104"/>
+      <c r="B1031" s="105"/>
+      <c r="C1031" s="106"/>
+      <c r="D1031" s="105"/>
+      <c r="E1031" s="105"/>
+    </row>
+    <row r="1032" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1032" s="104"/>
+      <c r="B1032" s="105"/>
+      <c r="C1032" s="106"/>
+      <c r="D1032" s="105"/>
+      <c r="E1032" s="105"/>
+    </row>
+    <row r="1033" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1033" s="104"/>
+      <c r="B1033" s="105"/>
+      <c r="C1033" s="106"/>
+      <c r="D1033" s="105"/>
+      <c r="E1033" s="105"/>
+    </row>
+    <row r="1034" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1034" s="104"/>
+      <c r="B1034" s="105"/>
+      <c r="C1034" s="106"/>
+      <c r="D1034" s="105"/>
+      <c r="E1034" s="105"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>